<commit_message>
Added Date Filter, Hid Cluster8, improved empty plot logic
</commit_message>
<xml_diff>
--- a/competencias.xlsx
+++ b/competencias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Ramirez\Desktop\Consultoria\Dashboards\CentroOrtopediaPoblado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448F745C-20F5-4E59-B117-93B9B58CD4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71151DC-AE17-454C-8D8C-F06E557855FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6D0F0DC0-A7B9-4FD1-A249-6D5F55889B05}"/>
+    <workbookView xWindow="35745" yWindow="1905" windowWidth="17340" windowHeight="12330" xr2:uid="{6D0F0DC0-A7B9-4FD1-A249-6D5F55889B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="109">
   <si>
     <t>Toma de Decisiones</t>
   </si>
@@ -297,15 +297,6 @@
   </si>
   <si>
     <t>Se mantiene al día con información de la competencia y las tendencias del mercado, identifican oportunidades de negocio para la organización, demuestra conocimiento financiero; controla costos y piensa en términos de beneficios, pérdidas y valor agregado.</t>
-  </si>
-  <si>
-    <t>Mantiene comunicación con los clientes actuales y busca crear nuevos contactos que posibiliten expandir el mercado.</t>
-  </si>
-  <si>
-    <t>Ha desarrollado habilidades de negociación que le permiten presentar propuestas comerciales que son acogidas favorablemente.</t>
-  </si>
-  <si>
-    <t>Se mantiene al día con la información de la competencia y las tendencias del mercado.</t>
   </si>
   <si>
     <t>Orientación al Servicio</t>
@@ -746,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601BDD1C-315F-498A-83CA-DB10B503864B}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,25 +752,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>97</v>
-      </c>
-      <c r="E1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -787,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -810,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -833,13 +824,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
@@ -856,7 +847,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -873,7 +864,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -896,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>21</v>
@@ -919,7 +910,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
@@ -942,7 +933,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>31</v>
@@ -965,7 +956,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>36</v>
@@ -988,7 +979,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>41</v>
@@ -1011,7 +1002,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>46</v>
@@ -1034,7 +1025,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>51</v>
@@ -1051,7 +1042,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>53</v>
@@ -1074,7 +1065,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>58</v>
@@ -1097,7 +1088,7 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>63</v>
@@ -1120,7 +1111,7 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>68</v>
@@ -1143,7 +1134,7 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>73</v>
@@ -1166,7 +1157,7 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>78</v>
@@ -1189,7 +1180,7 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>83</v>
@@ -1206,7 +1197,7 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>85</v>
@@ -1214,37 +1205,31 @@
       <c r="D21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>